<commit_message>
Corrected wrong fan link
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75195F8F-50D9-4B10-9777-25223218CDD0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0C6AE7-B194-47F4-9A4A-AFA39592BECD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>M3螺母</t>
   </si>
   <si>
-    <t>https://item.taobao.com/item.htm?spm=a1z09.2.0.0.23392e8d8E6i6H&amp;id=540751244209&amp;_u=a1ro9eu5ba6</t>
-  </si>
-  <si>
     <t>https://www.thingiverse.com/thing:2289203</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>https://au.mouser.com/ProductDetail/?qs=%2FW4LtXOBxKsfL3eA88psUg==</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z0k.6846577.0.0.6a306b8fzFQmZb&amp;id=551919051076&amp;_u=t2dmg8j26111</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -591,78 +591,78 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -670,13 +670,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,13 +684,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -698,16 +698,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -715,13 +715,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,16 +729,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,61 +746,61 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
         <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,10 +808,10 @@
     </row>
     <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -823,13 +823,13 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,27 +837,27 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,13 +865,13 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -879,52 +879,51 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" xr:uid="{07E1A463-A352-45B0-943C-146A9D54F6E9}"/>
-    <hyperlink ref="D12" r:id="rId2" xr:uid="{EF7CA771-432D-4D9B-8EA1-A98628D23401}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{CA3B6F12-E3E8-4E66-A549-4A79D6CA61E1}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{A41E13BD-F9FF-42AF-A977-5C3D7E467E54}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{2F345A83-1451-45EF-8637-CD3E06153E45}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{203A150F-E839-463F-A75E-C92433198615}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{E17262AD-4BD0-4A73-BE3F-F657C1CBCECF}"/>
-    <hyperlink ref="D13" r:id="rId8" xr:uid="{D35B66E1-32CD-46E7-A5FE-63BF1C0A26EA}"/>
-    <hyperlink ref="D20" r:id="rId9" xr:uid="{EC939544-3102-4371-9A30-4B98F6DF7DB7}"/>
-    <hyperlink ref="D21" r:id="rId10" xr:uid="{82767D4F-ADDE-4A64-B47C-23F84E41228A}"/>
-    <hyperlink ref="D22" r:id="rId11" xr:uid="{3240C3AF-12AB-4D8E-B6E5-CEBC6EB754BE}"/>
-    <hyperlink ref="D23" r:id="rId12" xr:uid="{70B2449B-6EEA-41A6-AFFA-907998FC0904}"/>
-    <hyperlink ref="D19" r:id="rId13" xr:uid="{B4077610-15BE-45B0-9802-EA924CBBA363}"/>
-    <hyperlink ref="D24" r:id="rId14" xr:uid="{8B4E2A89-3BCE-4525-A34F-241685ED8164}"/>
-    <hyperlink ref="D7" r:id="rId15" xr:uid="{9097859B-B4D6-4F01-B416-0FFF52C3462C}"/>
-    <hyperlink ref="D6" r:id="rId16" xr:uid="{A613CCEE-50A2-4056-821C-EB2CD810D710}"/>
-    <hyperlink ref="D16" r:id="rId17" xr:uid="{F9DF2F36-1598-4A05-A908-7F720A5A64CE}"/>
-    <hyperlink ref="F5" r:id="rId18" xr:uid="{841755F3-F9A3-4406-A6FA-97402ADAC88C}"/>
-    <hyperlink ref="D14" r:id="rId19" xr:uid="{B483143B-C1CC-4258-BAAD-0685D47DB152}"/>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{EF7CA771-432D-4D9B-8EA1-A98628D23401}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{CA3B6F12-E3E8-4E66-A549-4A79D6CA61E1}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{A41E13BD-F9FF-42AF-A977-5C3D7E467E54}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{2F345A83-1451-45EF-8637-CD3E06153E45}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{203A150F-E839-463F-A75E-C92433198615}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{E17262AD-4BD0-4A73-BE3F-F657C1CBCECF}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{D35B66E1-32CD-46E7-A5FE-63BF1C0A26EA}"/>
+    <hyperlink ref="D20" r:id="rId8" xr:uid="{EC939544-3102-4371-9A30-4B98F6DF7DB7}"/>
+    <hyperlink ref="D21" r:id="rId9" xr:uid="{82767D4F-ADDE-4A64-B47C-23F84E41228A}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{3240C3AF-12AB-4D8E-B6E5-CEBC6EB754BE}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{70B2449B-6EEA-41A6-AFFA-907998FC0904}"/>
+    <hyperlink ref="D19" r:id="rId12" xr:uid="{B4077610-15BE-45B0-9802-EA924CBBA363}"/>
+    <hyperlink ref="D24" r:id="rId13" xr:uid="{8B4E2A89-3BCE-4525-A34F-241685ED8164}"/>
+    <hyperlink ref="D7" r:id="rId14" xr:uid="{9097859B-B4D6-4F01-B416-0FFF52C3462C}"/>
+    <hyperlink ref="D6" r:id="rId15" xr:uid="{A613CCEE-50A2-4056-821C-EB2CD810D710}"/>
+    <hyperlink ref="D16" r:id="rId16" xr:uid="{F9DF2F36-1598-4A05-A908-7F720A5A64CE}"/>
+    <hyperlink ref="F5" r:id="rId17" xr:uid="{841755F3-F9A3-4406-A6FA-97402ADAC88C}"/>
+    <hyperlink ref="D14" r:id="rId18" xr:uid="{B483143B-C1CC-4258-BAAD-0685D47DB152}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 3510 fan link
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0C6AE7-B194-47F4-9A4A-AFA39592BECD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1403104-545A-4C37-B598-00C9B8EEE718}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <t>https://au.mouser.com/ProductDetail/?qs=%2FW4LtXOBxKsfL3eA88psUg==</t>
   </si>
   <si>
-    <t>https://item.taobao.com/item.htm?spm=a1z0k.6846577.0.0.6a306b8fzFQmZb&amp;id=551919051076&amp;_u=t2dmg8j26111</t>
+    <t>https://item.taobao.com/item.htm?spm=a1z0k.7386009.0.d4919233.447f7f62rI7wUe&amp;id=538704495777&amp;_u=t2dmg8j26111&amp;qq-pf-to=pcqq.group</t>
   </si>
 </sst>
 </file>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -922,8 +922,9 @@
     <hyperlink ref="D16" r:id="rId16" xr:uid="{F9DF2F36-1598-4A05-A908-7F720A5A64CE}"/>
     <hyperlink ref="F5" r:id="rId17" xr:uid="{841755F3-F9A3-4406-A6FA-97402ADAC88C}"/>
     <hyperlink ref="D14" r:id="rId18" xr:uid="{B483143B-C1CC-4258-BAAD-0685D47DB152}"/>
+    <hyperlink ref="F14" r:id="rId19" xr:uid="{7EB74423-7ED3-4646-89CF-957852A9596F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>